<commit_message>
wdk-opt + price done
</commit_message>
<xml_diff>
--- a/reports/Отчет 15-28.07.xlsx
+++ b/reports/Отчет 15-28.07.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Дата</t>
   </si>
@@ -41,6 +41,18 @@
   </si>
   <si>
     <t>Завершение оптимус, парсинг</t>
+  </si>
+  <si>
+    <t>Начало работы с ценами</t>
+  </si>
+  <si>
+    <t>Цены, проблема с форматом валют</t>
+  </si>
+  <si>
+    <t>Парсинг прайса донора в отдельные файлы WDK/OPT, ручное заполнение валют в новых прайсах (из-за того что в прайсе донора информация о валюте указана в виде формата внутри эксель вытянуть эту информацию автоматически не удалось)</t>
+  </si>
+  <si>
+    <t>Написание алгоритма и сопоставление двух прайсов с файлом выгрузки WDK/OPT с пометкой артикулов (OK/NOT FOUND)</t>
   </si>
 </sst>
 </file>
@@ -670,7 +682,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -783,13 +795,13 @@
         <v>45495</v>
       </c>
       <c r="B9" s="4">
-        <v>0.54166666666666663</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="C9" s="4">
         <v>0.6875</v>
       </c>
       <c r="D9" s="3">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>8</v>
@@ -802,36 +814,66 @@
       <c r="B10" s="4">
         <v>0.45833333333333331</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="7"/>
+      <c r="C10" s="4">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>45497</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B11" s="4">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="D11" s="3">
+        <v>2.25</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>45498</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="7"/>
+      <c r="B12" s="4">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.90625</v>
+      </c>
+      <c r="D12" s="3">
+        <v>2.75</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>45499</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="10"/>
+      <c r="B13" s="8">
+        <v>0.8125</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D13" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
@@ -862,7 +904,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1">
         <f>SUM(D2:D15)</f>
-        <v>10</v>
+        <v>19.5</v>
       </c>
       <c r="E17" s="1"/>
     </row>

</xml_diff>